<commit_message>
added notebooks, datacollection and chrome extension fix
</commit_message>
<xml_diff>
--- a/data/product recommendation query set.xlsx
+++ b/data/product recommendation query set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive\Desktop\Search vs Generation - A Comparative Study of Bing and ChatGPT in Product Recommendations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5368C712-E5B2-48D8-B11E-8EA1106D4E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D21D8C0-DF0E-479E-AA02-2982C21A57F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="3770" windowWidth="21900" windowHeight="15380" xr2:uid="{B28B15D7-B92C-4996-AB7A-16FAE932B28F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B28B15D7-B92C-4996-AB7A-16FAE932B28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,12 +110,6 @@
     <t>Electric Bicycle</t>
   </si>
   <si>
-    <t>Mirrorless Camera</t>
-  </si>
-  <si>
-    <t>Smart TV</t>
-  </si>
-  <si>
     <t>What is the best electric car?</t>
   </si>
   <si>
@@ -131,21 +125,6 @@
     <t>What is the best electric car under 50000 dollars with long range and fast charging?</t>
   </si>
   <si>
-    <t>What is the best mirrorless camera?</t>
-  </si>
-  <si>
-    <t>What is the best smart tv?</t>
-  </si>
-  <si>
-    <t>What is the best smart tv under 3000 dollars?</t>
-  </si>
-  <si>
-    <t>What is the best smart tv under 3000 dollars with 4k resolution?</t>
-  </si>
-  <si>
-    <t>What is the best smart tv under 3000 dollars with 4k resolution and high refresh rate?</t>
-  </si>
-  <si>
     <t>Drone</t>
   </si>
   <si>
@@ -212,15 +191,6 @@
     <t>What is the best smartwatch under 800 dollars with heart rate monitor and long battery life?</t>
   </si>
   <si>
-    <t>What is the best mirrorless camera under 3000 dollars?</t>
-  </si>
-  <si>
-    <t>What is the best mirrorless camera under 3000 dollars with fast autofocus?</t>
-  </si>
-  <si>
-    <t>What is the best mirrorless camera under 3000 dollars with fast autofocus and high resolution sensor?</t>
-  </si>
-  <si>
     <t>What is the best electric bicycle under 7500 dollars with good battery life?</t>
   </si>
   <si>
@@ -249,6 +219,36 @@
   </si>
   <si>
     <t>General &amp; Price &amp; Feature &amp; Feature</t>
+  </si>
+  <si>
+    <t>What is the best digital piano?</t>
+  </si>
+  <si>
+    <t>What is the best digital piano under 5000 dollars?</t>
+  </si>
+  <si>
+    <t>What is the best digital piano under 5000 dollars with weighted keys?</t>
+  </si>
+  <si>
+    <t>What is the best digital piano under 5000 dollars with weighted keys and Bluetooth connectivity?</t>
+  </si>
+  <si>
+    <t>Digital Piano</t>
+  </si>
+  <si>
+    <t>What is the best refrigerator?</t>
+  </si>
+  <si>
+    <t>What is the best refrigerator under 5000 dollars?</t>
+  </si>
+  <si>
+    <t>What is the best refrigerator under 5000 dollars with a built-in ice maker?</t>
+  </si>
+  <si>
+    <t>What is the best refrigerator under 5000 dollars with a built-in ice maker and smart Wi-Fi connectivity?</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
   </si>
 </sst>
 </file>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FF5BCB-6692-4302-89DA-FCDEB3C3B827}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,16 +633,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -667,10 +667,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -681,10 +681,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -695,10 +695,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -706,7 +706,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -720,13 +720,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -734,13 +734,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -748,13 +748,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -779,10 +779,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -793,10 +793,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -807,10 +807,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -835,10 +835,10 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -849,10 +849,10 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -863,10 +863,10 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -874,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -888,13 +888,13 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -902,13 +902,13 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -916,13 +916,13 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -930,7 +930,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -944,10 +944,10 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -958,10 +958,10 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -972,13 +972,13 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1003,7 +1003,7 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
@@ -1017,7 +1017,7 @@
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
@@ -1031,7 +1031,7 @@
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
         <v>18</v>
@@ -1059,10 +1059,10 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1073,10 +1073,10 @@
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1087,10 +1087,10 @@
         <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1104,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1115,10 +1115,10 @@
         <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -1129,10 +1129,10 @@
         <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D49" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1143,10 +1143,10 @@
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -1160,7 +1160,7 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1171,10 +1171,10 @@
         <v>23</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D53" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1185,10 +1185,10 @@
         <v>23</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -1199,10 +1199,10 @@
         <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1210,13 +1210,13 @@
         <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -1224,13 +1224,13 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D58" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1238,13 +1238,13 @@
         <v>21</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D59" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -1252,13 +1252,13 @@
         <v>21</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1266,13 +1266,13 @@
         <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1280,13 +1280,13 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D63" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -1294,13 +1294,13 @@
         <v>21</v>
       </c>
       <c r="B64" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D64" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -1308,13 +1308,13 @@
         <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D65" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>